<commit_message>
Filled in dates on SLR Dataset sheet
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/Covid_SLR_Dataset.xlsx
+++ b/Covid_19_Dataset_and_References/Covid_SLR_Dataset.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\2023USRAResearch\CovidClef2023\covidClef2023\Covid_19_Dataset_and_References\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9985F0CF-6E4F-4370-89ED-EA30AD70C6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="335">
   <si>
     <t>SLR Name</t>
   </si>
@@ -1018,55 +1027,84 @@
   <si>
     <t>https://docs.google.com/spreadsheets/d/1peHbijTfPxg6wVcBApZnDd4Uq1Nw8jhHw4sTUXOsFcI/edit#gid=0</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1074,7 +1112,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1084,58 +1122,53 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1325,20 +1358,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D112"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1348,1789 +1386,2127 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>334</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10">
+        <v>44075</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
+        <v>43942</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10">
+        <v>44042</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10">
+        <v>44105</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44005</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="10">
+        <v>44102</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44286</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="10">
+        <v>44286</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="10">
+        <v>44256</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="10">
+        <v>44224</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10">
+        <v>44397</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="10">
+        <v>44615</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="10">
+        <v>44809</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10">
+        <v>44280</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="10">
+        <v>44469</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="10">
+        <v>44621</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="10">
+        <v>44179</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="10">
+        <v>44125</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="10">
+        <v>44166</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C21" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10">
+        <v>44166</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C22" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="10">
+        <v>44079</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="10">
+        <v>43996</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="9" t="s">
         <v>71</v>
       </c>
       <c r="C24" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="E24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="10">
+        <v>43973</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="9" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="10">
+        <v>43983</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="10">
+        <v>44102</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C27" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="10">
+        <v>44044</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="9" t="s">
         <v>83</v>
       </c>
       <c r="C28" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="10">
+        <v>43920</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="10">
+        <v>44224</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30">
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C30" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="E30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="10">
+        <v>44133</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="10">
+        <v>44042</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="9" t="s">
         <v>94</v>
       </c>
       <c r="C32" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="10">
+        <v>44022</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C33" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="10">
+        <v>44015</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="9" t="s">
         <v>100</v>
       </c>
       <c r="C34" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="10">
+        <v>44011</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C35" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="10">
+        <v>44158</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C36" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10">
+        <v>44136</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C37" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="10">
+        <v>44138</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C38" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="10">
+        <v>44154</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="9" t="s">
         <v>115</v>
       </c>
       <c r="C39" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="10">
+        <v>44075</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C40" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="10">
+        <v>44064</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C41" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="10">
+        <v>44060</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C42" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="10">
+        <v>44322</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="9" t="s">
         <v>127</v>
       </c>
       <c r="C43" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="10">
+        <v>43999</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C44" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="10">
+        <v>44138</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C45" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="10">
+        <v>44652</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>134</v>
       </c>
       <c r="C46" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="10">
+        <v>44298</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C47" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="10">
+        <v>44025</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="9" t="s">
         <v>140</v>
       </c>
       <c r="C48" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E48" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="10">
+        <v>44126</v>
+      </c>
+      <c r="E48" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="9" t="s">
         <v>143</v>
       </c>
       <c r="C49" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="10">
+        <v>43983</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="9" t="s">
         <v>146</v>
       </c>
       <c r="C50" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="10">
+        <v>44228</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="9" t="s">
         <v>149</v>
       </c>
       <c r="C51" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="10">
+        <v>44487</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="3" t="s">
         <v>152</v>
       </c>
       <c r="C52" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="10">
+        <v>44415</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C53" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="10">
+        <v>44348</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C54" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="E54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="10">
+        <v>44182</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C55" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="10">
+        <v>44344</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="3" t="s">
         <v>164</v>
       </c>
       <c r="C56" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="10">
+        <v>44078</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C57" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="10">
+        <v>43963</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="3" t="s">
         <v>170</v>
       </c>
       <c r="C58" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="10">
+        <v>44085</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="9" t="s">
         <v>173</v>
       </c>
       <c r="C59" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="E59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="10">
+        <v>44083</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F59" s="11"/>
-    </row>
-    <row r="60">
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>176</v>
       </c>
       <c r="C60" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E60" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="10">
+        <v>44075</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="3" t="s">
         <v>179</v>
       </c>
       <c r="C61" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="10">
+        <v>44161</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="3" t="s">
         <v>182</v>
       </c>
       <c r="C62" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="10">
+        <v>44044</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="3" t="s">
         <v>185</v>
       </c>
       <c r="C63" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="10">
+        <v>44440</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="9" t="s">
         <v>188</v>
       </c>
       <c r="C64" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="E64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="10">
+        <v>44081</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="3" t="s">
         <v>191</v>
       </c>
       <c r="C65" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E65" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="10">
+        <v>44075</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C66" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="11">
+        <v>44250</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="9" t="s">
         <v>197</v>
       </c>
       <c r="C67" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="10">
+        <v>44409</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="3" t="s">
         <v>200</v>
       </c>
       <c r="C68" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E68" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="10">
+        <v>44410</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="3" t="s">
         <v>203</v>
       </c>
       <c r="C69" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="E69" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="10">
+        <v>44265</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C70" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="10">
+        <v>44409</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C71" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="E71" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="10">
+        <v>44238</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="9" t="s">
         <v>212</v>
       </c>
       <c r="C72" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="10">
+        <v>44004</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="9" t="s">
         <v>215</v>
       </c>
       <c r="C73" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E73" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="10">
+        <v>44372</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="9" t="s">
         <v>218</v>
       </c>
       <c r="C74" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="E74" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="10">
+        <v>44378</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="3" t="s">
         <v>221</v>
       </c>
       <c r="C75" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="E75" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="10">
+        <v>44106</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="9" t="s">
         <v>224</v>
       </c>
       <c r="C76" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E76" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="10">
+        <v>44101</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="9" t="s">
         <v>227</v>
       </c>
       <c r="C77" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E77" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="10">
+        <v>44235</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="9" t="s">
         <v>230</v>
       </c>
       <c r="C78" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E78" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="10">
+        <v>44138</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="9" t="s">
         <v>233</v>
       </c>
       <c r="C79" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="10">
+        <v>44155</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="3" t="s">
         <v>236</v>
       </c>
       <c r="C80" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E80" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="10">
+        <v>44120</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="3" t="s">
         <v>239</v>
       </c>
       <c r="C81" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="E81" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="10">
+        <v>44376</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="3" t="s">
         <v>242</v>
       </c>
       <c r="C82" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E82" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="10">
+        <v>44090</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="3" t="s">
         <v>245</v>
       </c>
       <c r="C83" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E83" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="10">
+        <v>44351</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="9" t="s">
         <v>248</v>
       </c>
       <c r="C84" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E84" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="10">
+        <v>44163</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="3" t="s">
         <v>251</v>
       </c>
       <c r="C85" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="E85" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" s="10">
+        <v>44678</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="9" t="s">
         <v>254</v>
       </c>
       <c r="C86" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E86" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="10">
+        <v>44197</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="3" t="s">
         <v>257</v>
       </c>
       <c r="C87" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E87" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="10">
+        <v>45030</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="3" t="s">
         <v>260</v>
       </c>
       <c r="C88" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E88" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="10">
+        <v>44043</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="9" t="s">
         <v>263</v>
       </c>
       <c r="C89" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E89" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="10">
+        <v>44319</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="9" t="s">
         <v>266</v>
       </c>
       <c r="C90" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E90" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="10">
+        <v>44196</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="3" t="s">
         <v>269</v>
       </c>
       <c r="C91" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="E91" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="10">
+        <v>44128</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="3" t="s">
         <v>272</v>
       </c>
       <c r="C92" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E92" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="10">
+        <v>44197</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="9" t="s">
         <v>275</v>
       </c>
       <c r="C93" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E93" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="10">
+        <v>44127</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="3" t="s">
         <v>278</v>
       </c>
       <c r="C94" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E94" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" s="10">
+        <v>44336</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C95" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E95" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="10">
+        <v>44365</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C96" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E96" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="10">
+        <v>44244</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="9" t="s">
         <v>287</v>
       </c>
       <c r="C97" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E97" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97" s="10">
+        <v>44080</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="9" t="s">
         <v>290</v>
       </c>
       <c r="C98" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E98" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" s="10">
+        <v>44363</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="3" t="s">
         <v>293</v>
       </c>
       <c r="C99" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E99" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" s="10">
+        <v>44187</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="3" t="s">
         <v>296</v>
       </c>
       <c r="C100" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E100" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" s="10">
+        <v>44132</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="3" t="s">
         <v>299</v>
       </c>
       <c r="C101" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="E101" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="10">
+        <v>44061</v>
+      </c>
+      <c r="E101" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="3" t="s">
         <v>302</v>
       </c>
       <c r="C102" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E102" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="10">
+        <v>44370</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="3" t="s">
         <v>305</v>
       </c>
       <c r="C103" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E103" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" s="10">
+        <v>44345</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="3" t="s">
         <v>308</v>
       </c>
       <c r="C104" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E104" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104" s="10">
+        <v>44368</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="3" t="s">
         <v>311</v>
       </c>
       <c r="C105" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E105" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D105" s="10">
+        <v>44201</v>
+      </c>
+      <c r="E105" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="3" t="s">
         <v>314</v>
       </c>
       <c r="C106" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E106" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D106" s="10">
+        <v>44361</v>
+      </c>
+      <c r="E106" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="3" t="s">
         <v>317</v>
       </c>
       <c r="C107" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="E107" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" s="10">
+        <v>44228</v>
+      </c>
+      <c r="E107" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="3" t="s">
         <v>320</v>
       </c>
       <c r="C108" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E108" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="10">
+        <v>44136</v>
+      </c>
+      <c r="E108" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="3" t="s">
         <v>323</v>
       </c>
       <c r="C109" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="E109" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" s="10">
+        <v>44463</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="3" t="s">
         <v>326</v>
       </c>
       <c r="C110" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E110" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D110" s="10">
+        <v>44180</v>
+      </c>
+      <c r="E110" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="9" t="s">
         <v>329</v>
       </c>
       <c r="C111" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E111" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111" s="10">
+        <v>44309</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="3" t="s">
         <v>332</v>
       </c>
       <c r="C112" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E112" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="10">
+        <v>44334</v>
+      </c>
+      <c r="E112" s="2" t="s">
         <v>333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" location="gid=0" ref="E2"/>
-    <hyperlink r:id="rId2" location="gid=0" ref="E3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" location="gid=0" ref="E4"/>
-    <hyperlink r:id="rId5" ref="B5"/>
-    <hyperlink r:id="rId6" location="gid=0" ref="E5"/>
-    <hyperlink r:id="rId7" ref="B6"/>
-    <hyperlink r:id="rId8" ref="E6"/>
-    <hyperlink r:id="rId9" ref="B7"/>
-    <hyperlink r:id="rId10" location="gid=0" ref="E7"/>
-    <hyperlink r:id="rId11" ref="B8"/>
-    <hyperlink r:id="rId12" location="gid=0" ref="E8"/>
-    <hyperlink r:id="rId13" ref="B9"/>
-    <hyperlink r:id="rId14" location="gid=0" ref="E9"/>
-    <hyperlink r:id="rId15" ref="B10"/>
-    <hyperlink r:id="rId16" location="gid=0" ref="E10"/>
-    <hyperlink r:id="rId17" ref="B11"/>
-    <hyperlink r:id="rId18" ref="E11"/>
-    <hyperlink r:id="rId19" ref="B12"/>
-    <hyperlink r:id="rId20" location="gid=0" ref="E12"/>
-    <hyperlink r:id="rId21" location=":~:text=The%20meta%2Danalysis%20showed%20that,%2D0.88%5D%2C%20P%20%3C%20." ref="B13"/>
-    <hyperlink r:id="rId22" location="gid=0" ref="E13"/>
-    <hyperlink r:id="rId23" ref="B14"/>
-    <hyperlink r:id="rId24" location="gid=0" ref="E14"/>
-    <hyperlink r:id="rId25" ref="B15"/>
-    <hyperlink r:id="rId26" location="gid=0" ref="E15"/>
-    <hyperlink r:id="rId27" ref="B16"/>
-    <hyperlink r:id="rId28" location="gid=0" ref="E16"/>
-    <hyperlink r:id="rId29" ref="B17"/>
-    <hyperlink r:id="rId30" location="gid=0" ref="E17"/>
-    <hyperlink r:id="rId31" ref="B18"/>
-    <hyperlink r:id="rId32" location="gid=0" ref="E18"/>
-    <hyperlink r:id="rId33" ref="B19"/>
-    <hyperlink r:id="rId34" location="gid=0" ref="E19"/>
-    <hyperlink r:id="rId35" ref="B20"/>
-    <hyperlink r:id="rId36" location="gid=0" ref="E20"/>
-    <hyperlink r:id="rId37" ref="B21"/>
-    <hyperlink r:id="rId38" location="gid=0" ref="E21"/>
-    <hyperlink r:id="rId39" location="!/" ref="B22"/>
-    <hyperlink r:id="rId40" location="gid=0" ref="E22"/>
-    <hyperlink r:id="rId41" ref="B23"/>
-    <hyperlink r:id="rId42" location="gid=0" ref="E23"/>
-    <hyperlink r:id="rId43" ref="B24"/>
-    <hyperlink r:id="rId44" location="gid=0" ref="E24"/>
-    <hyperlink r:id="rId45" location=":~:text=Conclusion%3A%20It%20is%20uncertain%20whether,rapid%20need%20for%20further%20studies." ref="B25"/>
-    <hyperlink r:id="rId46" location="gid=0" ref="E25"/>
-    <hyperlink r:id="rId47" ref="B26"/>
-    <hyperlink r:id="rId48" location="gid=0" ref="E26"/>
-    <hyperlink r:id="rId49" ref="B27"/>
-    <hyperlink r:id="rId50" location="gid=0" ref="E27"/>
-    <hyperlink r:id="rId51" ref="B28"/>
-    <hyperlink r:id="rId52" location="gid=0" ref="E28"/>
-    <hyperlink r:id="rId53" ref="B29"/>
-    <hyperlink r:id="rId54" location="gid=0" ref="E29"/>
-    <hyperlink r:id="rId55" ref="B30"/>
-    <hyperlink r:id="rId56" location="gid=0" ref="E30"/>
-    <hyperlink r:id="rId57" ref="B31"/>
-    <hyperlink r:id="rId58" location="gid=0" ref="E31"/>
-    <hyperlink r:id="rId59" ref="B32"/>
-    <hyperlink r:id="rId60" location="gid=0" ref="E32"/>
-    <hyperlink r:id="rId61" ref="B33"/>
-    <hyperlink r:id="rId62" location="gid=0" ref="E33"/>
-    <hyperlink r:id="rId63" ref="B34"/>
-    <hyperlink r:id="rId64" location="gid=0" ref="E34"/>
-    <hyperlink r:id="rId65" ref="B35"/>
-    <hyperlink r:id="rId66" location="gid=0" ref="E35"/>
-    <hyperlink r:id="rId67" ref="B36"/>
-    <hyperlink r:id="rId68" location="gid=0" ref="E36"/>
-    <hyperlink r:id="rId69" ref="B37"/>
-    <hyperlink r:id="rId70" location="gid=0" ref="E37"/>
-    <hyperlink r:id="rId71" ref="B38"/>
-    <hyperlink r:id="rId72" location="gid=0" ref="E38"/>
-    <hyperlink r:id="rId73" ref="B39"/>
-    <hyperlink r:id="rId74" location="gid=0" ref="E39"/>
-    <hyperlink r:id="rId75" ref="B40"/>
-    <hyperlink r:id="rId76" location="gid=0" ref="E40"/>
-    <hyperlink r:id="rId77" ref="B41"/>
-    <hyperlink r:id="rId78" location="gid=0" ref="E41"/>
-    <hyperlink r:id="rId79" ref="B42"/>
-    <hyperlink r:id="rId80" location="gid=0" ref="E42"/>
-    <hyperlink r:id="rId81" ref="B43"/>
-    <hyperlink r:id="rId82" location="gid=0" ref="E43"/>
-    <hyperlink r:id="rId83" ref="B44"/>
-    <hyperlink r:id="rId84" location="gid=0" ref="E44"/>
-    <hyperlink r:id="rId85" ref="B45"/>
-    <hyperlink r:id="rId86" location="gid=0" ref="E45"/>
-    <hyperlink r:id="rId87" ref="B46"/>
-    <hyperlink r:id="rId88" location="gid=0" ref="E46"/>
-    <hyperlink r:id="rId89" ref="B47"/>
-    <hyperlink r:id="rId90" location="gid=0" ref="E47"/>
-    <hyperlink r:id="rId91" ref="B48"/>
-    <hyperlink r:id="rId92" location="gid=0" ref="E48"/>
-    <hyperlink r:id="rId93" ref="B49"/>
-    <hyperlink r:id="rId94" location="gid=0" ref="E49"/>
-    <hyperlink r:id="rId95" ref="B50"/>
-    <hyperlink r:id="rId96" location="gid=0" ref="E50"/>
-    <hyperlink r:id="rId97" ref="B51"/>
-    <hyperlink r:id="rId98" location="gid=0" ref="E51"/>
-    <hyperlink r:id="rId99" ref="B52"/>
-    <hyperlink r:id="rId100" location="gid=0" ref="E52"/>
-    <hyperlink r:id="rId101" ref="B53"/>
-    <hyperlink r:id="rId102" location="gid=0" ref="E53"/>
-    <hyperlink r:id="rId103" ref="B54"/>
-    <hyperlink r:id="rId104" location="gid=0" ref="E54"/>
-    <hyperlink r:id="rId105" ref="B55"/>
-    <hyperlink r:id="rId106" location="gid=0" ref="E55"/>
-    <hyperlink r:id="rId107" ref="B56"/>
-    <hyperlink r:id="rId108" location="gid=0" ref="E56"/>
-    <hyperlink r:id="rId109" ref="B57"/>
-    <hyperlink r:id="rId110" location="gid=0" ref="E57"/>
-    <hyperlink r:id="rId111" ref="B58"/>
-    <hyperlink r:id="rId112" location="gid=0" ref="E58"/>
-    <hyperlink r:id="rId113" ref="B59"/>
-    <hyperlink r:id="rId114" location="gid=0" ref="E59"/>
-    <hyperlink r:id="rId115" ref="B60"/>
-    <hyperlink r:id="rId116" location="gid=0" ref="E60"/>
-    <hyperlink r:id="rId117" ref="B61"/>
-    <hyperlink r:id="rId118" location="gid=0" ref="E61"/>
-    <hyperlink r:id="rId119" ref="B62"/>
-    <hyperlink r:id="rId120" location="gid=0" ref="E62"/>
-    <hyperlink r:id="rId121" ref="B63"/>
-    <hyperlink r:id="rId122" location="gid=0" ref="E63"/>
-    <hyperlink r:id="rId123" ref="B64"/>
-    <hyperlink r:id="rId124" location="gid=0" ref="E64"/>
-    <hyperlink r:id="rId125" ref="B65"/>
-    <hyperlink r:id="rId126" location="gid=0" ref="E65"/>
-    <hyperlink r:id="rId127" ref="B66"/>
-    <hyperlink r:id="rId128" location="gid=0" ref="E66"/>
-    <hyperlink r:id="rId129" ref="B67"/>
-    <hyperlink r:id="rId130" location="gid=0" ref="E67"/>
-    <hyperlink r:id="rId131" ref="B68"/>
-    <hyperlink r:id="rId132" location="gid=0" ref="E68"/>
-    <hyperlink r:id="rId133" ref="B69"/>
-    <hyperlink r:id="rId134" location="gid=0" ref="E69"/>
-    <hyperlink r:id="rId135" ref="B70"/>
-    <hyperlink r:id="rId136" location="gid=0" ref="E70"/>
-    <hyperlink r:id="rId137" ref="B71"/>
-    <hyperlink r:id="rId138" location="gid=0" ref="E71"/>
-    <hyperlink r:id="rId139" ref="B72"/>
-    <hyperlink r:id="rId140" location="gid=0" ref="E72"/>
-    <hyperlink r:id="rId141" ref="B73"/>
-    <hyperlink r:id="rId142" location="gid=0" ref="E73"/>
-    <hyperlink r:id="rId143" ref="B74"/>
-    <hyperlink r:id="rId144" location="gid=0" ref="E74"/>
-    <hyperlink r:id="rId145" ref="B75"/>
-    <hyperlink r:id="rId146" location="gid=0" ref="E75"/>
-    <hyperlink r:id="rId147" ref="B76"/>
-    <hyperlink r:id="rId148" location="gid=0" ref="E76"/>
-    <hyperlink r:id="rId149" ref="B77"/>
-    <hyperlink r:id="rId150" location="gid=0" ref="E77"/>
-    <hyperlink r:id="rId151" ref="B78"/>
-    <hyperlink r:id="rId152" location="gid=0" ref="E78"/>
-    <hyperlink r:id="rId153" ref="B79"/>
-    <hyperlink r:id="rId154" location="gid=0" ref="E79"/>
-    <hyperlink r:id="rId155" ref="B80"/>
-    <hyperlink r:id="rId156" location="gid=0" ref="E80"/>
-    <hyperlink r:id="rId157" ref="B81"/>
-    <hyperlink r:id="rId158" location="gid=0" ref="E81"/>
-    <hyperlink r:id="rId159" ref="B82"/>
-    <hyperlink r:id="rId160" location="gid=0" ref="E82"/>
-    <hyperlink r:id="rId161" ref="B83"/>
-    <hyperlink r:id="rId162" location="gid=0" ref="E83"/>
-    <hyperlink r:id="rId163" ref="B84"/>
-    <hyperlink r:id="rId164" location="gid=0" ref="E84"/>
-    <hyperlink r:id="rId165" ref="B85"/>
-    <hyperlink r:id="rId166" location="gid=0" ref="E85"/>
-    <hyperlink r:id="rId167" ref="B86"/>
-    <hyperlink r:id="rId168" location="gid=0" ref="E86"/>
-    <hyperlink r:id="rId169" ref="B87"/>
-    <hyperlink r:id="rId170" location="gid=0" ref="E87"/>
-    <hyperlink r:id="rId171" ref="B88"/>
-    <hyperlink r:id="rId172" location="gid=0" ref="E88"/>
-    <hyperlink r:id="rId173" ref="B89"/>
-    <hyperlink r:id="rId174" location="gid=0" ref="E89"/>
-    <hyperlink r:id="rId175" ref="B90"/>
-    <hyperlink r:id="rId176" location="gid=0" ref="E90"/>
-    <hyperlink r:id="rId177" ref="B91"/>
-    <hyperlink r:id="rId178" location="gid=0" ref="E91"/>
-    <hyperlink r:id="rId179" ref="B92"/>
-    <hyperlink r:id="rId180" location="gid=0" ref="E92"/>
-    <hyperlink r:id="rId181" ref="B93"/>
-    <hyperlink r:id="rId182" location="gid=0" ref="E93"/>
-    <hyperlink r:id="rId183" ref="B94"/>
-    <hyperlink r:id="rId184" location="gid=0" ref="E94"/>
-    <hyperlink r:id="rId185" ref="B95"/>
-    <hyperlink r:id="rId186" location="gid=0" ref="E95"/>
-    <hyperlink r:id="rId187" ref="B96"/>
-    <hyperlink r:id="rId188" location="gid=0" ref="E96"/>
-    <hyperlink r:id="rId189" ref="B97"/>
-    <hyperlink r:id="rId190" location="gid=0" ref="E97"/>
-    <hyperlink r:id="rId191" ref="B98"/>
-    <hyperlink r:id="rId192" location="gid=0" ref="E98"/>
-    <hyperlink r:id="rId193" ref="B99"/>
-    <hyperlink r:id="rId194" location="gid=0" ref="E99"/>
-    <hyperlink r:id="rId195" ref="B100"/>
-    <hyperlink r:id="rId196" location="gid=0" ref="E100"/>
-    <hyperlink r:id="rId197" ref="B101"/>
-    <hyperlink r:id="rId198" location="gid=0" ref="E101"/>
-    <hyperlink r:id="rId199" ref="B102"/>
-    <hyperlink r:id="rId200" location="gid=0" ref="E102"/>
-    <hyperlink r:id="rId201" ref="B103"/>
-    <hyperlink r:id="rId202" location="gid=0" ref="E103"/>
-    <hyperlink r:id="rId203" ref="B104"/>
-    <hyperlink r:id="rId204" location="gid=0" ref="E104"/>
-    <hyperlink r:id="rId205" ref="B105"/>
-    <hyperlink r:id="rId206" location="gid=0" ref="E105"/>
-    <hyperlink r:id="rId207" location="citeas" ref="B106"/>
-    <hyperlink r:id="rId208" location="gid=0" ref="E106"/>
-    <hyperlink r:id="rId209" ref="B107"/>
-    <hyperlink r:id="rId210" location="gid=0" ref="E107"/>
-    <hyperlink r:id="rId211" ref="B108"/>
-    <hyperlink r:id="rId212" location="gid=0" ref="E108"/>
-    <hyperlink r:id="rId213" ref="B109"/>
-    <hyperlink r:id="rId214" location="gid=0" ref="E109"/>
-    <hyperlink r:id="rId215" ref="B110"/>
-    <hyperlink r:id="rId216" location="gid=0" ref="E110"/>
-    <hyperlink r:id="rId217" ref="B111"/>
-    <hyperlink r:id="rId218" location="gid=0" ref="E111"/>
-    <hyperlink r:id="rId219" ref="B112"/>
-    <hyperlink r:id="rId220" location="gid=0" ref="E112"/>
+    <hyperlink ref="E2" r:id="rId1" location="gid=0" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" location="gid=0" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E4" r:id="rId4" location="gid=0" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E5" r:id="rId6" location="gid=0" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E7" r:id="rId10" location="gid=0" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E8" r:id="rId12" location="gid=0" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E9" r:id="rId14" location="gid=0" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E10" r:id="rId16" location="gid=0" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E12" r:id="rId20" location="gid=0" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B13" r:id="rId21" location=":~:text=The%20meta%2Danalysis%20showed%20that,%2D0.88%5D%2C%20P%20%3C%20." xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E13" r:id="rId22" location="gid=0" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B14" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E14" r:id="rId24" location="gid=0" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B15" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E15" r:id="rId26" location="gid=0" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B16" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E16" r:id="rId28" location="gid=0" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B17" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E17" r:id="rId30" location="gid=0" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B18" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E18" r:id="rId32" location="gid=0" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B19" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E19" r:id="rId34" location="gid=0" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B20" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E20" r:id="rId36" location="gid=0" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B21" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E21" r:id="rId38" location="gid=0" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B22" r:id="rId39" location="!/" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E22" r:id="rId40" location="gid=0" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B23" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E23" r:id="rId42" location="gid=0" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B24" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E24" r:id="rId44" location="gid=0" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B25" r:id="rId45" location=":~:text=Conclusion%3A%20It%20is%20uncertain%20whether,rapid%20need%20for%20further%20studies." xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E25" r:id="rId46" location="gid=0" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B26" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E26" r:id="rId48" location="gid=0" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B27" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E27" r:id="rId50" location="gid=0" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B28" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E28" r:id="rId52" location="gid=0" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B29" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="E29" r:id="rId54" location="gid=0" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B30" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="E30" r:id="rId56" location="gid=0" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B31" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="E31" r:id="rId58" location="gid=0" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B32" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="E32" r:id="rId60" location="gid=0" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B33" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="E33" r:id="rId62" location="gid=0" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B34" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="E34" r:id="rId64" location="gid=0" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B35" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="E35" r:id="rId66" location="gid=0" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B36" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="E36" r:id="rId68" location="gid=0" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B37" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="E37" r:id="rId70" location="gid=0" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B38" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="E38" r:id="rId72" location="gid=0" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B39" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="E39" r:id="rId74" location="gid=0" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B40" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="E40" r:id="rId76" location="gid=0" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B41" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="E41" r:id="rId78" location="gid=0" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B42" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="E42" r:id="rId80" location="gid=0" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B43" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="E43" r:id="rId82" location="gid=0" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B44" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="E44" r:id="rId84" location="gid=0" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B45" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="E45" r:id="rId86" location="gid=0" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B46" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="E46" r:id="rId88" location="gid=0" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B47" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="E47" r:id="rId90" location="gid=0" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B48" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="E48" r:id="rId92" location="gid=0" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B49" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="E49" r:id="rId94" location="gid=0" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B50" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="E50" r:id="rId96" location="gid=0" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B51" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="E51" r:id="rId98" location="gid=0" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B52" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="E52" r:id="rId100" location="gid=0" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B53" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="E53" r:id="rId102" location="gid=0" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B54" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="E54" r:id="rId104" location="gid=0" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B55" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="E55" r:id="rId106" location="gid=0" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B56" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="E56" r:id="rId108" location="gid=0" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B57" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="E57" r:id="rId110" location="gid=0" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B58" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="E58" r:id="rId112" location="gid=0" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B59" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="E59" r:id="rId114" location="gid=0" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B60" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="E60" r:id="rId116" location="gid=0" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B61" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="E61" r:id="rId118" location="gid=0" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B62" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="E62" r:id="rId120" location="gid=0" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B63" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="E63" r:id="rId122" location="gid=0" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B64" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="E64" r:id="rId124" location="gid=0" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B65" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="E65" r:id="rId126" location="gid=0" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B66" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="E66" r:id="rId128" location="gid=0" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B67" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="E67" r:id="rId130" location="gid=0" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B68" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="E68" r:id="rId132" location="gid=0" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B69" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="E69" r:id="rId134" location="gid=0" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B70" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="E70" r:id="rId136" location="gid=0" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B71" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="E71" r:id="rId138" location="gid=0" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B72" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="E72" r:id="rId140" location="gid=0" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B73" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="E73" r:id="rId142" location="gid=0" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B74" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="E74" r:id="rId144" location="gid=0" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B75" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="E75" r:id="rId146" location="gid=0" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B76" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="E76" r:id="rId148" location="gid=0" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B77" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="E77" r:id="rId150" location="gid=0" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B78" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="E78" r:id="rId152" location="gid=0" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B79" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="E79" r:id="rId154" location="gid=0" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B80" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="E80" r:id="rId156" location="gid=0" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B81" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="E81" r:id="rId158" location="gid=0" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B82" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="E82" r:id="rId160" location="gid=0" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B83" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="E83" r:id="rId162" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B84" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="E84" r:id="rId164" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B85" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="E85" r:id="rId166" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B86" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="E86" r:id="rId168" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B87" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="E87" r:id="rId170" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B88" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="E88" r:id="rId172" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B89" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="E89" r:id="rId174" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="B90" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="E90" r:id="rId176" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="B91" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="E91" r:id="rId178" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="B92" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="E92" r:id="rId180" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="B93" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="E93" r:id="rId182" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="B94" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="E94" r:id="rId184" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="B95" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="E95" r:id="rId186" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="B96" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="E96" r:id="rId188" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="B97" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="E97" r:id="rId190" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="B98" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="E98" r:id="rId192" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="B99" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="E99" r:id="rId194" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="B100" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="E100" r:id="rId196" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="B101" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="E101" r:id="rId198" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="B102" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="E102" r:id="rId200" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="B103" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="E103" r:id="rId202" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="B104" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="E104" r:id="rId204" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="B105" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="E105" r:id="rId206" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="B106" r:id="rId207" location="citeas" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="E106" r:id="rId208" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="B107" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="E107" r:id="rId210" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="B108" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="E108" r:id="rId212" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="B109" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="E109" r:id="rId214" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="B110" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="E110" r:id="rId216" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="B111" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="E111" r:id="rId218" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="B112" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="E112" r:id="rId220" location="gid=0" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="B3" r:id="rId221" xr:uid="{ACB9792D-7EB0-421B-8E55-29310E480861}"/>
   </hyperlinks>
-  <drawing r:id="rId221"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId222"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dated Search Added, qrel changes finalized
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/Covid_SLR_Dataset.xlsx
+++ b/Covid_19_Dataset_and_References/Covid_SLR_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\2023USRAResearch\CovidClef2023\covidClef2023\Covid_19_Dataset_and_References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9985F0CF-6E4F-4370-89ED-EA30AD70C6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6079411-8EB8-4957-9B5C-FCC0D4B6112C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,7 +1036,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1147,8 +1147,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1371,7 +1371,7 @@
   <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D112"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1427,7 +1427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>67</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>82</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>102</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>108</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>111</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>114</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>120</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>126</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>108</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>130</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>133</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>136</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>139</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>142</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>145</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>148</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>151</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>154</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>157</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>160</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>163</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>166</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>169</v>
       </c>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>175</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>178</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>181</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>184</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>190</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>199</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>202</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>205</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>208</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>220</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>235</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>238</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>241</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>244</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>250</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>256</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>259</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>268</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>271</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>277</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>280</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>283</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>292</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>295</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>298</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>301</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>304</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>307</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>310</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>313</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>316</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>319</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>322</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>325</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>331</v>
       </c>

</xml_diff>

<commit_message>
added the chatgpt based queries for the SLR topics.
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/Covid_SLR_Dataset.xlsx
+++ b/Covid_19_Dataset_and_References/Covid_SLR_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\2023USRAResearch\CovidClef2023\covidClef2023\Covid_19_Dataset_and_References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1724D185-1F1E-4F96-91FE-4C75B760170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF71D23-48C1-4914-BACA-386FBA2A5FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="725">
   <si>
     <t>SLR Name</t>
   </si>
@@ -1996,9 +1996,6 @@
   </si>
   <si>
     <t>Global Seasonality of Human Seasonal Coronaviruses: A Clue for Postpandemic Circulating Season of Severe Acute Respiratory Syndrome Coronavirus 2?</t>
-  </si>
-  <si>
-    <t>########</t>
   </si>
   <si>
     <t>Background
@@ -3392,6 +3389,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3555,21 +3555,12 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3595,6 +3586,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4009,10 +4009,13 @@
   <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -4050,31 +4053,31 @@
       <c r="A2" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="16">
+        <v>44075</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>335</v>
       </c>
       <c r="G2" s="2">
         <v>7454715</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>561</v>
       </c>
     </row>
@@ -4082,19 +4085,19 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="16">
+        <v>43942</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>336</v>
       </c>
       <c r="G3" s="2">
@@ -4112,31 +4115,31 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="16">
+        <v>44042</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>337</v>
       </c>
       <c r="G4" s="2">
         <v>7393956</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>562</v>
       </c>
     </row>
@@ -4144,31 +4147,31 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="16">
+        <v>44105</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>338</v>
       </c>
       <c r="G5" s="2">
         <v>7577386</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>563</v>
       </c>
     </row>
@@ -4176,31 +4179,31 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="16">
+        <v>44005</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>339</v>
       </c>
       <c r="G6" s="2">
         <v>7331754</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>564</v>
       </c>
     </row>
@@ -4208,19 +4211,19 @@
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="16">
+        <v>44102</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>340</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -4229,7 +4232,7 @@
       <c r="H7" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>535</v>
       </c>
       <c r="J7" s="1"/>
@@ -4238,31 +4241,31 @@
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="16">
+        <v>44286</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>341</v>
       </c>
       <c r="G8" s="2">
         <v>8013817</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>565</v>
       </c>
     </row>
@@ -4270,31 +4273,31 @@
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="16">
+        <v>44286</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>342</v>
       </c>
       <c r="G9" s="2">
         <v>8011308</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>566</v>
       </c>
     </row>
@@ -4302,31 +4305,31 @@
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="2">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="16">
+        <v>44256</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>343</v>
       </c>
       <c r="G10" s="2">
         <v>7917447</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>567</v>
       </c>
     </row>
@@ -4334,31 +4337,31 @@
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="16">
+        <v>44224</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>344</v>
       </c>
       <c r="G11" s="2">
         <v>7876291</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>568</v>
       </c>
     </row>
@@ -4366,26 +4369,26 @@
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="16">
+        <v>44397</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>345</v>
       </c>
       <c r="G12" s="2">
         <v>8291630</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>452</v>
@@ -4398,31 +4401,31 @@
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="2">
         <v>6</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="16">
+        <v>44615</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>346</v>
       </c>
       <c r="G13" s="2">
         <v>9111510</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>570</v>
       </c>
     </row>
@@ -4430,26 +4433,26 @@
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="2">
         <v>4</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="16">
+        <v>44809</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>347</v>
       </c>
       <c r="G14" s="2">
         <v>9599062</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>454</v>
@@ -4462,26 +4465,26 @@
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="16">
+        <v>44280</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>348</v>
       </c>
       <c r="G15" s="2">
         <v>7993905</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>455</v>
@@ -4494,19 +4497,19 @@
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="2">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="16">
+        <v>44469</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>349</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -4515,7 +4518,7 @@
       <c r="H16" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>537</v>
       </c>
       <c r="J16" s="1"/>
@@ -4524,31 +4527,31 @@
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="2">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D17" s="16">
+        <v>44621</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>350</v>
       </c>
       <c r="G17" s="2">
         <v>8817946</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>573</v>
       </c>
     </row>
@@ -4556,26 +4559,26 @@
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="2">
         <v>3</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="16">
+        <v>44179</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>351</v>
       </c>
       <c r="G18" s="2">
         <v>7735177</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>457</v>
@@ -4588,19 +4591,19 @@
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="2">
         <v>3</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="16">
+        <v>44125</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>352</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -4609,8 +4612,8 @@
       <c r="H19" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>646</v>
+      <c r="I19" s="8" t="s">
+        <v>645</v>
       </c>
       <c r="J19" s="1"/>
     </row>
@@ -4618,27 +4621,27 @@
       <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="16">
+        <v>44166</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="1" t="s">
         <v>438</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>647</v>
+      <c r="I20" s="3" t="s">
+        <v>646</v>
       </c>
       <c r="J20" s="1"/>
     </row>
@@ -4646,31 +4649,31 @@
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="2">
         <v>3</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="16">
+        <v>44166</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G21" s="2">
         <v>9404081</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>574</v>
       </c>
     </row>
@@ -4678,26 +4681,26 @@
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C22" s="2">
         <v>2</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="16">
+        <v>44079</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>353</v>
       </c>
       <c r="G22" s="2">
         <v>7537484</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>459</v>
@@ -4710,16 +4713,16 @@
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C23" s="2">
         <v>2</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="16">
+        <v>43996</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>68</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -4731,8 +4734,8 @@
       <c r="H23" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>651</v>
+      <c r="I23" s="9" t="s">
+        <v>650</v>
       </c>
       <c r="J23" s="1"/>
     </row>
@@ -4740,31 +4743,31 @@
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="2">
         <v>21</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="16">
+        <v>43973</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>355</v>
       </c>
       <c r="G24" s="2">
         <v>7281716</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="3" t="s">
         <v>576</v>
       </c>
     </row>
@@ -4772,26 +4775,26 @@
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="2">
         <v>4</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="16">
+        <v>43983</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>356</v>
       </c>
       <c r="G25" s="2">
         <v>7169929</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>461</v>
@@ -4804,31 +4807,31 @@
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="2">
         <v>6</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" s="16">
+        <v>44102</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>357</v>
       </c>
       <c r="G26" s="2">
         <v>7836759</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="3" t="s">
         <v>578</v>
       </c>
     </row>
@@ -4836,19 +4839,19 @@
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C27" s="2">
         <v>5</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="16">
+        <v>44044</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="10" t="s">
         <v>358</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -4857,7 +4860,7 @@
       <c r="H27" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="3" t="s">
         <v>542</v>
       </c>
       <c r="J27" s="1"/>
@@ -4866,31 +4869,31 @@
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="2">
         <v>5</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="D28" s="16">
+        <v>43920</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>359</v>
       </c>
       <c r="G28" s="2">
         <v>7230636</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="3" t="s">
         <v>579</v>
       </c>
     </row>
@@ -4898,31 +4901,31 @@
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C29" s="2">
         <v>4</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="D29" s="16">
+        <v>44224</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="11" t="s">
         <v>360</v>
       </c>
       <c r="G29" s="2">
         <v>7884669</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="3" t="s">
         <v>580</v>
       </c>
     </row>
@@ -4930,19 +4933,19 @@
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="2">
         <v>7</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="D30" s="16">
+        <v>44133</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>361</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -4951,8 +4954,8 @@
       <c r="H30" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>657</v>
+      <c r="I30" s="3" t="s">
+        <v>656</v>
       </c>
       <c r="J30" s="1"/>
     </row>
@@ -4960,31 +4963,31 @@
       <c r="A31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="2">
         <v>3</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E31" s="6" t="s">
+      <c r="D31" s="16">
+        <v>44042</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>337</v>
       </c>
       <c r="G31" s="2">
         <v>7393956</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="3" t="s">
         <v>562</v>
       </c>
     </row>
@@ -4992,26 +4995,26 @@
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="2">
         <v>3</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="D32" s="16">
+        <v>44022</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>362</v>
       </c>
       <c r="G32" s="2">
         <v>7351172</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>466</v>
@@ -5024,31 +5027,31 @@
       <c r="A33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C33" s="2">
         <v>4</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="D33" s="16">
+        <v>44015</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>363</v>
       </c>
       <c r="G33" s="2">
         <v>7350605</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="3" t="s">
         <v>581</v>
       </c>
     </row>
@@ -5056,19 +5059,19 @@
       <c r="A34" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C34" s="2">
         <v>5</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="D34" s="16">
+        <v>44011</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="12" t="s">
         <v>364</v>
       </c>
       <c r="G34" s="2">
@@ -5078,7 +5081,7 @@
       <c r="I34" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="J34" s="3" t="s">
         <v>582</v>
       </c>
     </row>
@@ -5086,31 +5089,31 @@
       <c r="A35" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C35" s="2">
         <v>4</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="D35" s="16">
+        <v>44158</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="12" t="s">
         <v>365</v>
       </c>
       <c r="G35" s="2">
         <v>7682759</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="3" t="s">
         <v>583</v>
       </c>
     </row>
@@ -5118,19 +5121,19 @@
       <c r="A36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C36" s="2">
         <v>3</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="D36" s="16">
+        <v>44136</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="5" t="s">
         <v>366</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -5139,8 +5142,8 @@
       <c r="H36" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>661</v>
+      <c r="I36" s="6" t="s">
+        <v>660</v>
       </c>
       <c r="J36" s="1"/>
     </row>
@@ -5148,26 +5151,26 @@
       <c r="A37" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C37" s="2">
         <v>3</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E37" s="6" t="s">
+      <c r="D37" s="16">
+        <v>44138</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="5" t="s">
         <v>367</v>
       </c>
       <c r="G37" s="2">
         <v>7608886</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>470</v>
@@ -5180,31 +5183,31 @@
       <c r="A38" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C38" s="2">
         <v>6</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="D38" s="16">
+        <v>44154</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>368</v>
       </c>
       <c r="G38" s="2">
         <v>7674121</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="J38" s="3" t="s">
         <v>584</v>
       </c>
     </row>
@@ -5212,31 +5215,31 @@
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C39" s="2">
         <v>3</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E39" s="6" t="s">
+      <c r="D39" s="16">
+        <v>44075</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="5" t="s">
         <v>369</v>
       </c>
       <c r="G39" s="2">
         <v>7337824</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="J39" s="3" t="s">
         <v>585</v>
       </c>
     </row>
@@ -5244,31 +5247,31 @@
       <c r="A40" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>117</v>
       </c>
       <c r="C40" s="2">
         <v>6</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="D40" s="16">
+        <v>44064</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>370</v>
       </c>
       <c r="G40" s="2">
         <v>7441862</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J40" s="3" t="s">
         <v>586</v>
       </c>
     </row>
@@ -5276,28 +5279,28 @@
       <c r="A41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>120</v>
       </c>
       <c r="C41" s="2">
         <v>4</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="D41" s="16">
+        <v>44060</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>371</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>438</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="I41" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>545</v>
       </c>
       <c r="J41" s="1"/>
@@ -5306,31 +5309,31 @@
       <c r="A42" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C42" s="2">
         <v>5</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="D42" s="16">
+        <v>44322</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="5" t="s">
         <v>372</v>
       </c>
       <c r="G42" s="2">
         <v>8207055</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="J42" s="3" t="s">
         <v>587</v>
       </c>
     </row>
@@ -5338,20 +5341,20 @@
       <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C43" s="2">
         <v>4</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E43" s="6" t="s">
+      <c r="D43" s="16">
+        <v>43999</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F43" s="6" t="s">
-        <v>668</v>
+      <c r="F43" s="5" t="s">
+        <v>667</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>438</v>
@@ -5359,8 +5362,8 @@
       <c r="H43" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="I43" s="4" t="s">
-        <v>669</v>
+      <c r="I43" s="3" t="s">
+        <v>668</v>
       </c>
       <c r="J43" s="1"/>
     </row>
@@ -5368,26 +5371,26 @@
       <c r="A44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C44" s="2">
         <v>3</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E44" s="6" t="s">
+      <c r="D44" s="16">
+        <v>44138</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F44" s="5" t="s">
         <v>367</v>
       </c>
       <c r="G44" s="2">
         <v>7608886</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>475</v>
@@ -5400,31 +5403,31 @@
       <c r="A45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C45" s="2">
         <v>3</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E45" s="6" t="s">
+      <c r="D45" s="16">
+        <v>44652</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="5" t="s">
         <v>373</v>
       </c>
       <c r="G45" s="2">
         <v>10012754</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="J45" s="3" t="s">
         <v>588</v>
       </c>
     </row>
@@ -5432,31 +5435,31 @@
       <c r="A46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C46" s="2">
         <v>5</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E46" s="6" t="s">
+      <c r="D46" s="16">
+        <v>44298</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="11" t="s">
         <v>374</v>
       </c>
       <c r="G46" s="2">
         <v>8060540</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J46" s="3" t="s">
         <v>589</v>
       </c>
     </row>
@@ -5464,31 +5467,31 @@
       <c r="A47" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>136</v>
       </c>
       <c r="C47" s="2">
         <v>6</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E47" s="6" t="s">
+      <c r="D47" s="16">
+        <v>44025</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="5" t="s">
         <v>375</v>
       </c>
       <c r="G47" s="2">
         <v>8302895</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J47" s="3" t="s">
         <v>590</v>
       </c>
     </row>
@@ -5496,31 +5499,31 @@
       <c r="A48" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C48" s="2">
         <v>3</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E48" s="10" t="s">
+      <c r="D48" s="16">
+        <v>44126</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F48" s="5" t="s">
         <v>376</v>
       </c>
       <c r="G48" s="2">
         <v>7582054</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="3" t="s">
         <v>591</v>
       </c>
     </row>
@@ -5528,16 +5531,16 @@
       <c r="A49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C49" s="2">
         <v>3</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E49" s="6" t="s">
+      <c r="D49" s="16">
+        <v>43983</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F49" s="1" t="s">
@@ -5547,12 +5550,12 @@
         <v>7484929</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="J49" s="3" t="s">
         <v>592</v>
       </c>
     </row>
@@ -5560,31 +5563,31 @@
       <c r="A50" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>145</v>
       </c>
       <c r="C50" s="2">
         <v>5</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E50" s="6" t="s">
+      <c r="D50" s="16">
+        <v>44228</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="5" t="s">
         <v>380</v>
       </c>
       <c r="G50" s="2">
         <v>7764387</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J50" s="3" t="s">
         <v>593</v>
       </c>
     </row>
@@ -5592,16 +5595,16 @@
       <c r="A51" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>148</v>
       </c>
       <c r="C51" s="2">
         <v>4</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E51" s="6" t="s">
+      <c r="D51" s="16">
+        <v>44487</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>149</v>
       </c>
       <c r="F51" s="1" t="s">
@@ -5620,31 +5623,31 @@
       <c r="A52" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C52" s="2">
         <v>4</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E52" s="6" t="s">
+      <c r="D52" s="16">
+        <v>44415</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F52" s="5" t="s">
         <v>382</v>
       </c>
       <c r="G52" s="2">
         <v>8363901</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="J52" s="3" t="s">
         <v>594</v>
       </c>
     </row>
@@ -5652,31 +5655,31 @@
       <c r="A53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>154</v>
       </c>
       <c r="C53" s="2">
         <v>5</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E53" s="6" t="s">
+      <c r="D53" s="16">
+        <v>44348</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="5" t="s">
         <v>383</v>
       </c>
       <c r="G53" s="2">
         <v>8164188</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J53" s="3" t="s">
         <v>595</v>
       </c>
     </row>
@@ -5684,31 +5687,31 @@
       <c r="A54" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>157</v>
       </c>
       <c r="C54" s="2">
         <v>11</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E54" s="6" t="s">
+      <c r="D54" s="16">
+        <v>44182</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="4" t="s">
         <v>384</v>
       </c>
       <c r="G54" s="2">
         <v>7746770</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="J54" s="3" t="s">
         <v>596</v>
       </c>
     </row>
@@ -5716,26 +5719,26 @@
       <c r="A55" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>160</v>
       </c>
       <c r="C55" s="2">
         <v>5</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E55" s="6" t="s">
+      <c r="D55" s="16">
+        <v>44344</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F55" s="5" t="s">
         <v>385</v>
       </c>
       <c r="G55" s="2">
         <v>8166456</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>485</v>
@@ -5748,19 +5751,19 @@
       <c r="A56" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>163</v>
       </c>
       <c r="C56" s="2">
         <v>5</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E56" s="6" t="s">
+      <c r="D56" s="16">
+        <v>44078</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="F56" s="5" t="s">
         <v>386</v>
       </c>
       <c r="G56" s="1" t="s">
@@ -5769,7 +5772,7 @@
       <c r="H56" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="I56" s="4" t="s">
+      <c r="I56" s="3" t="s">
         <v>548</v>
       </c>
       <c r="J56" s="1"/>
@@ -5778,31 +5781,31 @@
       <c r="A57" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>166</v>
       </c>
       <c r="C57" s="2">
         <v>4</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E57" s="6" t="s">
+      <c r="D57" s="16">
+        <v>43963</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F57" s="5" t="s">
         <v>387</v>
       </c>
       <c r="G57" s="2">
         <v>7217103</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="J57" s="4" t="s">
+      <c r="J57" s="3" t="s">
         <v>566</v>
       </c>
     </row>
@@ -5810,19 +5813,19 @@
       <c r="A58" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="5" t="s">
         <v>169</v>
       </c>
       <c r="C58" s="2">
         <v>6</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E58" s="6" t="s">
+      <c r="D58" s="16">
+        <v>44085</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F58" s="6" t="s">
+      <c r="F58" s="5" t="s">
         <v>378</v>
       </c>
       <c r="G58" s="2">
@@ -5832,7 +5835,7 @@
       <c r="I58" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="J58" s="3" t="s">
         <v>598</v>
       </c>
     </row>
@@ -5840,31 +5843,31 @@
       <c r="A59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>172</v>
       </c>
       <c r="C59" s="2">
         <v>7</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E59" s="6" t="s">
+      <c r="D59" s="16">
+        <v>44083</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="F59" s="6" t="s">
+      <c r="F59" s="5" t="s">
         <v>388</v>
       </c>
       <c r="G59" s="2">
         <v>7510504</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="J59" s="3" t="s">
         <v>599</v>
       </c>
     </row>
@@ -5872,31 +5875,31 @@
       <c r="A60" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>175</v>
       </c>
       <c r="C60" s="2">
         <v>4</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E60" s="6" t="s">
+      <c r="D60" s="16">
+        <v>44075</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="F60" s="5" t="s">
         <v>388</v>
       </c>
       <c r="G60" s="2">
         <v>7510504</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="J60" s="3" t="s">
         <v>599</v>
       </c>
     </row>
@@ -5904,31 +5907,31 @@
       <c r="A61" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>178</v>
       </c>
       <c r="C61" s="2">
         <v>6</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E61" s="6" t="s">
+      <c r="D61" s="16">
+        <v>44161</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="4" t="s">
         <v>389</v>
       </c>
       <c r="G61" s="2">
         <v>7691365</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="J61" s="3" t="s">
         <v>596</v>
       </c>
     </row>
@@ -5936,19 +5939,19 @@
       <c r="A62" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="5" t="s">
         <v>181</v>
       </c>
       <c r="C62" s="2">
         <v>4</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E62" s="6" t="s">
+      <c r="D62" s="16">
+        <v>44044</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="F62" s="5" t="s">
         <v>390</v>
       </c>
       <c r="G62" s="2">
@@ -5966,26 +5969,26 @@
       <c r="A63" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>184</v>
       </c>
       <c r="C63" s="2">
         <v>3</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E63" s="6" t="s">
+      <c r="D63" s="16">
+        <v>44440</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="F63" s="5" t="s">
         <v>391</v>
       </c>
       <c r="G63" s="2">
         <v>8233909</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>492</v>
@@ -5998,31 +6001,31 @@
       <c r="A64" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="5" t="s">
         <v>187</v>
       </c>
       <c r="C64" s="2">
         <v>8</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E64" s="6" t="s">
+      <c r="D64" s="16">
+        <v>44081</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F64" s="11" t="s">
         <v>392</v>
       </c>
       <c r="G64" s="2">
         <v>7487805</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="J64" s="4" t="s">
+      <c r="J64" s="3" t="s">
         <v>602</v>
       </c>
     </row>
@@ -6030,31 +6033,31 @@
       <c r="A65" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="5" t="s">
         <v>190</v>
       </c>
       <c r="C65" s="2">
         <v>2</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E65" s="6" t="s">
+      <c r="D65" s="16">
+        <v>44075</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="F65" s="5" t="s">
         <v>393</v>
       </c>
       <c r="G65" s="2">
         <v>7239135</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="J65" s="4" t="s">
+      <c r="J65" s="3" t="s">
         <v>603</v>
       </c>
     </row>
@@ -6062,16 +6065,16 @@
       <c r="A66" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="5" t="s">
         <v>193</v>
       </c>
       <c r="C66" s="2">
         <v>3</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E66" s="6" t="s">
+      <c r="D66" s="16">
+        <v>44250</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>194</v>
       </c>
       <c r="F66" s="1" t="s">
@@ -6083,7 +6086,7 @@
       <c r="H66" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="I66" s="4" t="s">
+      <c r="I66" s="3" t="s">
         <v>550</v>
       </c>
       <c r="J66" s="1"/>
@@ -6092,31 +6095,31 @@
       <c r="A67" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="5" t="s">
         <v>196</v>
       </c>
       <c r="C67" s="2">
         <v>2</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E67" s="6" t="s">
+      <c r="D67" s="16">
+        <v>44409</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="F67" s="6" t="s">
+      <c r="F67" s="5" t="s">
         <v>395</v>
       </c>
       <c r="G67" s="2">
         <v>8298932</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="J67" s="4" t="s">
+      <c r="J67" s="3" t="s">
         <v>567</v>
       </c>
     </row>
@@ -6124,31 +6127,31 @@
       <c r="A68" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="5" t="s">
         <v>199</v>
       </c>
       <c r="C68" s="2">
         <v>2</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E68" s="6" t="s">
+      <c r="D68" s="16">
+        <v>44410</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="F68" s="5" t="s">
         <v>379</v>
       </c>
       <c r="G68" s="2">
         <v>8420453</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="J68" s="4" t="s">
+      <c r="J68" s="3" t="s">
         <v>604</v>
       </c>
     </row>
@@ -6156,26 +6159,26 @@
       <c r="A69" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="5" t="s">
         <v>202</v>
       </c>
       <c r="C69" s="2">
         <v>11</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E69" s="6" t="s">
+      <c r="D69" s="16">
+        <v>44265</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="F69" s="5" t="s">
         <v>396</v>
       </c>
       <c r="G69" s="2">
         <v>7946321</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>497</v>
@@ -6188,19 +6191,19 @@
       <c r="A70" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="5" t="s">
         <v>205</v>
       </c>
       <c r="C70" s="2">
         <v>2</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E70" s="6" t="s">
+      <c r="D70" s="16">
+        <v>44409</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="F70" s="5" t="s">
         <v>397</v>
       </c>
       <c r="G70" s="2">
@@ -6210,7 +6213,7 @@
       <c r="I70" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="J70" s="4" t="s">
+      <c r="J70" s="3" t="s">
         <v>605</v>
       </c>
     </row>
@@ -6218,16 +6221,16 @@
       <c r="A71" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="5" t="s">
         <v>208</v>
       </c>
       <c r="C71" s="2">
         <v>10</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E71" s="6" t="s">
+      <c r="D71" s="16">
+        <v>44238</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>209</v>
       </c>
       <c r="F71" s="1" t="s">
@@ -6237,7 +6240,7 @@
         <v>7877631</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>499</v>
@@ -6250,31 +6253,31 @@
       <c r="A72" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
         <v>211</v>
       </c>
       <c r="C72" s="2">
         <v>5</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E72" s="6" t="s">
+      <c r="D72" s="16">
+        <v>44004</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="F72" s="5" t="s">
         <v>402</v>
       </c>
       <c r="G72" s="2">
         <v>7310609</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="J72" s="4" t="s">
+      <c r="J72" s="3" t="s">
         <v>606</v>
       </c>
     </row>
@@ -6282,26 +6285,26 @@
       <c r="A73" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C73" s="2">
         <v>1</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E73" s="6" t="s">
+      <c r="D73" s="16">
+        <v>44372</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F73" s="6" t="s">
+      <c r="F73" s="5" t="s">
         <v>403</v>
       </c>
       <c r="G73" s="2">
         <v>8233054</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>501</v>
@@ -6314,31 +6317,31 @@
       <c r="A74" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="5" t="s">
         <v>217</v>
       </c>
       <c r="C74" s="2">
         <v>10</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E74" s="6" t="s">
+      <c r="D74" s="16">
+        <v>44378</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="F74" s="5" t="s">
         <v>404</v>
       </c>
       <c r="G74" s="2">
         <v>9225824</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="J74" s="4" t="s">
+      <c r="J74" s="3" t="s">
         <v>608</v>
       </c>
     </row>
@@ -6346,31 +6349,31 @@
       <c r="A75" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="5" t="s">
         <v>220</v>
       </c>
       <c r="C75" s="2">
         <v>9</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E75" s="6" t="s">
+      <c r="D75" s="16">
+        <v>44106</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="F75" s="6" t="s">
+      <c r="F75" s="5" t="s">
         <v>405</v>
       </c>
       <c r="G75" s="2">
         <v>7675607</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="J75" s="3" t="s">
         <v>609</v>
       </c>
     </row>
@@ -6378,26 +6381,26 @@
       <c r="A76" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="5" t="s">
         <v>223</v>
       </c>
       <c r="C76" s="2">
         <v>3</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E76" s="6" t="s">
+      <c r="D76" s="16">
+        <v>44101</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="F76" s="6" t="s">
+      <c r="F76" s="5" t="s">
         <v>406</v>
       </c>
       <c r="G76" s="2">
         <v>7599513</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>504</v>
@@ -6410,19 +6413,19 @@
       <c r="A77" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="5" t="s">
         <v>226</v>
       </c>
       <c r="C77" s="2">
         <v>3</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E77" s="6" t="s">
+      <c r="D77" s="16">
+        <v>44235</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="F77" s="6" t="s">
+      <c r="F77" s="5" t="s">
         <v>407</v>
       </c>
       <c r="G77" s="1" t="s">
@@ -6431,7 +6434,7 @@
       <c r="H77" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="I77" s="3" t="s">
         <v>552</v>
       </c>
       <c r="J77" s="1"/>
@@ -6440,26 +6443,26 @@
       <c r="A78" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="5" t="s">
         <v>229</v>
       </c>
       <c r="C78" s="2">
         <v>4</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E78" s="6" t="s">
+      <c r="D78" s="16">
+        <v>44138</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="F78" s="6" t="s">
+      <c r="F78" s="5" t="s">
         <v>399</v>
       </c>
       <c r="G78" s="2">
         <v>7608911</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>505</v>
@@ -6472,26 +6475,26 @@
       <c r="A79" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="5" t="s">
         <v>232</v>
       </c>
       <c r="C79" s="2">
         <v>6</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E79" s="6" t="s">
+      <c r="D79" s="16">
+        <v>44155</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="F79" s="6" t="s">
+      <c r="F79" s="5" t="s">
         <v>400</v>
       </c>
       <c r="G79" s="2">
         <v>7678983</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>506</v>
@@ -6504,31 +6507,31 @@
       <c r="A80" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="5" t="s">
         <v>235</v>
       </c>
       <c r="C80" s="2">
         <v>6</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E80" s="6" t="s">
+      <c r="D80" s="16">
+        <v>44120</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="F80" s="6" t="s">
+      <c r="F80" s="5" t="s">
         <v>409</v>
       </c>
       <c r="G80" s="2">
         <v>7566758</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="J80" s="4" t="s">
+      <c r="J80" s="3" t="s">
         <v>611</v>
       </c>
     </row>
@@ -6536,26 +6539,26 @@
       <c r="A81" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="5" t="s">
         <v>238</v>
       </c>
       <c r="C81" s="2">
         <v>8</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E81" s="6" t="s">
+      <c r="D81" s="16">
+        <v>44376</v>
+      </c>
+      <c r="E81" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="F81" s="6" t="s">
+      <c r="F81" s="5" t="s">
         <v>401</v>
       </c>
       <c r="G81" s="2">
         <v>8241122</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>508</v>
@@ -6568,16 +6571,16 @@
       <c r="A82" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="5" t="s">
         <v>241</v>
       </c>
       <c r="C82" s="2">
         <v>6</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E82" s="6" t="s">
+      <c r="D82" s="16">
+        <v>44090</v>
+      </c>
+      <c r="E82" s="5" t="s">
         <v>242</v>
       </c>
       <c r="F82" s="1" t="s">
@@ -6598,26 +6601,26 @@
       <c r="A83" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="5" t="s">
         <v>244</v>
       </c>
       <c r="C83" s="2">
         <v>3</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E83" s="6" t="s">
+      <c r="D83" s="16">
+        <v>44351</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F83" s="6" t="s">
+      <c r="F83" s="5" t="s">
         <v>408</v>
       </c>
       <c r="G83" s="2">
         <v>8177443</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>509</v>
@@ -6630,31 +6633,31 @@
       <c r="A84" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B84" s="5" t="s">
         <v>247</v>
       </c>
       <c r="C84" s="2">
         <v>4</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E84" s="6" t="s">
+      <c r="D84" s="16">
+        <v>44163</v>
+      </c>
+      <c r="E84" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="F84" s="6" t="s">
+      <c r="F84" s="5" t="s">
         <v>411</v>
       </c>
       <c r="G84" s="2">
         <v>7698829</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="J84" s="4" t="s">
+      <c r="J84" s="3" t="s">
         <v>612</v>
       </c>
     </row>
@@ -6662,31 +6665,31 @@
       <c r="A85" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="5" t="s">
         <v>250</v>
       </c>
       <c r="C85" s="2">
         <v>14</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E85" s="6" t="s">
+      <c r="D85" s="16">
+        <v>44678</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F85" s="6" t="s">
+      <c r="F85" s="5" t="s">
         <v>412</v>
       </c>
       <c r="G85" s="2">
         <v>7771023</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="J85" s="3" t="s">
         <v>613</v>
       </c>
     </row>
@@ -6694,31 +6697,31 @@
       <c r="A86" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="5" t="s">
         <v>253</v>
       </c>
       <c r="C86" s="2">
         <v>5</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E86" s="6" t="s">
+      <c r="D86" s="16">
+        <v>44197</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="F86" s="6" t="s">
+      <c r="F86" s="5" t="s">
         <v>413</v>
       </c>
       <c r="G86" s="2">
         <v>9183207</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="J86" s="4" t="s">
+      <c r="J86" s="3" t="s">
         <v>614</v>
       </c>
     </row>
@@ -6726,16 +6729,16 @@
       <c r="A87" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="5" t="s">
         <v>256</v>
       </c>
       <c r="C87" s="2">
         <v>6</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E87" s="6" t="s">
+      <c r="D87" s="16">
+        <v>45030</v>
+      </c>
+      <c r="E87" s="5" t="s">
         <v>257</v>
       </c>
       <c r="F87" s="1" t="s">
@@ -6754,31 +6757,31 @@
       <c r="A88" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B88" s="5" t="s">
         <v>259</v>
       </c>
       <c r="C88" s="2">
         <v>5</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E88" s="6" t="s">
+      <c r="D88" s="16">
+        <v>44043</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="F88" s="6" t="s">
+      <c r="F88" s="5" t="s">
         <v>414</v>
       </c>
       <c r="G88" s="2">
         <v>7528540</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="J88" s="4" t="s">
+      <c r="J88" s="3" t="s">
         <v>615</v>
       </c>
     </row>
@@ -6786,26 +6789,26 @@
       <c r="A89" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="5" t="s">
         <v>262</v>
       </c>
       <c r="C89" s="2">
         <v>2</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E89" s="6" t="s">
+      <c r="D89" s="16">
+        <v>44319</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F89" s="6" t="s">
+      <c r="F89" s="5" t="s">
         <v>415</v>
       </c>
       <c r="G89" s="2">
         <v>8098961</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>514</v>
@@ -6818,19 +6821,19 @@
       <c r="A90" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="5" t="s">
         <v>265</v>
       </c>
       <c r="C90" s="2">
         <v>4</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E90" s="6" t="s">
+      <c r="D90" s="16">
+        <v>44196</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="F90" s="6" t="s">
+      <c r="F90" s="5" t="s">
         <v>416</v>
       </c>
       <c r="G90" s="2">
@@ -6848,31 +6851,31 @@
       <c r="A91" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="5" t="s">
         <v>268</v>
       </c>
       <c r="C91" s="2">
         <v>8</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E91" s="6" t="s">
+      <c r="D91" s="16">
+        <v>44128</v>
+      </c>
+      <c r="E91" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="F91" s="6" t="s">
+      <c r="F91" s="5" t="s">
         <v>417</v>
       </c>
       <c r="G91" s="2">
         <v>7698263</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="J91" s="3" t="s">
         <v>616</v>
       </c>
     </row>
@@ -6880,31 +6883,31 @@
       <c r="A92" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="5" t="s">
         <v>271</v>
       </c>
       <c r="C92" s="2">
         <v>3</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E92" s="6" t="s">
+      <c r="D92" s="16">
+        <v>44197</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="F92" s="6" t="s">
+      <c r="F92" s="5" t="s">
         <v>418</v>
       </c>
       <c r="G92" s="2">
         <v>7495188</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="J92" s="3" t="s">
         <v>617</v>
       </c>
     </row>
@@ -6912,28 +6915,28 @@
       <c r="A93" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="5" t="s">
         <v>274</v>
       </c>
       <c r="C93" s="2">
         <v>3</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E93" s="6" t="s">
+      <c r="D93" s="16">
+        <v>44127</v>
+      </c>
+      <c r="E93" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="F93" s="6" t="s">
+      <c r="F93" s="5" t="s">
         <v>419</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="H93" s="16" t="s">
-        <v>707</v>
-      </c>
-      <c r="I93" s="4" t="s">
+      <c r="H93" s="13" t="s">
+        <v>706</v>
+      </c>
+      <c r="I93" s="3" t="s">
         <v>555</v>
       </c>
       <c r="J93" s="1"/>
@@ -6942,31 +6945,31 @@
       <c r="A94" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B94" s="5" t="s">
         <v>277</v>
       </c>
       <c r="C94" s="2">
         <v>3</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E94" s="6" t="s">
+      <c r="D94" s="16">
+        <v>44336</v>
+      </c>
+      <c r="E94" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F94" s="6" t="s">
+      <c r="F94" s="5" t="s">
         <v>420</v>
       </c>
       <c r="G94" s="2">
         <v>8135192</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="J94" s="4" t="s">
+      <c r="J94" s="3" t="s">
         <v>618</v>
       </c>
     </row>
@@ -6974,28 +6977,28 @@
       <c r="A95" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="5" t="s">
         <v>280</v>
       </c>
       <c r="C95" s="2">
         <v>6</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E95" s="6" t="s">
+      <c r="D95" s="16">
+        <v>44365</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F95" s="6" t="s">
+      <c r="F95" s="5" t="s">
         <v>421</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="H95" s="5" t="s">
+      <c r="H95" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="I95" s="4" t="s">
+      <c r="I95" s="3" t="s">
         <v>557</v>
       </c>
       <c r="J95" s="1"/>
@@ -7004,31 +7007,31 @@
       <c r="A96" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B96" s="5" t="s">
         <v>283</v>
       </c>
       <c r="C96" s="2">
         <v>6</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E96" s="6" t="s">
+      <c r="D96" s="16">
+        <v>44244</v>
+      </c>
+      <c r="E96" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="F96" s="6" t="s">
+      <c r="F96" s="5" t="s">
         <v>422</v>
       </c>
       <c r="G96" s="2">
         <v>7926203</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="J96" s="3" t="s">
         <v>564</v>
       </c>
     </row>
@@ -7036,31 +7039,31 @@
       <c r="A97" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B97" s="5" t="s">
         <v>286</v>
       </c>
       <c r="C97" s="2">
         <v>3</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E97" s="6" t="s">
+      <c r="D97" s="16">
+        <v>44080</v>
+      </c>
+      <c r="E97" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F97" s="6" t="s">
+      <c r="F97" s="5" t="s">
         <v>423</v>
       </c>
       <c r="G97" s="2">
         <v>7476422</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="J97" s="4" t="s">
+      <c r="J97" s="3" t="s">
         <v>619</v>
       </c>
     </row>
@@ -7068,31 +7071,31 @@
       <c r="A98" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B98" s="6" t="s">
+      <c r="B98" s="5" t="s">
         <v>289</v>
       </c>
       <c r="C98" s="2">
         <v>4</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E98" s="6" t="s">
+      <c r="D98" s="16">
+        <v>44363</v>
+      </c>
+      <c r="E98" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="F98" s="6" t="s">
+      <c r="F98" s="5" t="s">
         <v>424</v>
       </c>
       <c r="G98" s="2">
         <v>8205550</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="J98" s="4" t="s">
+      <c r="J98" s="3" t="s">
         <v>620</v>
       </c>
     </row>
@@ -7100,31 +7103,31 @@
       <c r="A99" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="B99" s="5" t="s">
         <v>292</v>
       </c>
       <c r="C99" s="2">
         <v>3</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E99" s="6" t="s">
+      <c r="D99" s="16">
+        <v>44187</v>
+      </c>
+      <c r="E99" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="F99" s="15" t="s">
+      <c r="F99" s="12" t="s">
         <v>425</v>
       </c>
       <c r="G99" s="2">
         <v>7753517</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="J99" s="4" t="s">
+      <c r="J99" s="3" t="s">
         <v>621</v>
       </c>
     </row>
@@ -7132,26 +7135,26 @@
       <c r="A100" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="B100" s="5" t="s">
         <v>295</v>
       </c>
       <c r="C100" s="2">
         <v>4</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E100" s="6" t="s">
+      <c r="D100" s="16">
+        <v>44132</v>
+      </c>
+      <c r="E100" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F100" s="6" t="s">
+      <c r="F100" s="5" t="s">
         <v>426</v>
       </c>
       <c r="G100" s="2">
         <v>7598542</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>522</v>
@@ -7164,31 +7167,31 @@
       <c r="A101" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B101" s="5" t="s">
         <v>298</v>
       </c>
       <c r="C101" s="2">
         <v>8</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E101" s="6" t="s">
+      <c r="D101" s="16">
+        <v>44061</v>
+      </c>
+      <c r="E101" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="F101" s="6" t="s">
+      <c r="F101" s="5" t="s">
         <v>427</v>
       </c>
       <c r="G101" s="2">
         <v>7461373</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="J101" s="4" t="s">
+      <c r="J101" s="3" t="s">
         <v>622</v>
       </c>
     </row>
@@ -7196,26 +7199,26 @@
       <c r="A102" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B102" s="5" t="s">
         <v>301</v>
       </c>
       <c r="C102" s="2">
         <v>5</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E102" s="6" t="s">
+      <c r="D102" s="16">
+        <v>44370</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="F102" s="6" t="s">
+      <c r="F102" s="5" t="s">
         <v>428</v>
       </c>
       <c r="G102" s="2">
         <v>8221462</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>524</v>
@@ -7228,31 +7231,31 @@
       <c r="A103" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B103" s="5" t="s">
         <v>304</v>
       </c>
       <c r="C103" s="2">
         <v>2</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E103" s="6" t="s">
+      <c r="D103" s="16">
+        <v>44345</v>
+      </c>
+      <c r="E103" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="F103" s="15" t="s">
+      <c r="F103" s="12" t="s">
         <v>429</v>
       </c>
       <c r="G103" s="2">
         <v>8164261</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="J103" s="4" t="s">
+      <c r="J103" s="3" t="s">
         <v>623</v>
       </c>
     </row>
@@ -7260,20 +7263,20 @@
       <c r="A104" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B104" s="5" t="s">
         <v>307</v>
       </c>
       <c r="C104" s="2">
         <v>3</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E104" s="6" t="s">
+      <c r="D104" s="16">
+        <v>44368</v>
+      </c>
+      <c r="E104" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F104" s="6" t="s">
-        <v>717</v>
+      <c r="F104" s="5" t="s">
+        <v>716</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>438</v>
@@ -7281,7 +7284,7 @@
       <c r="H104" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="I104" s="4" t="s">
+      <c r="I104" s="3" t="s">
         <v>559</v>
       </c>
       <c r="J104" s="1"/>
@@ -7290,31 +7293,31 @@
       <c r="A105" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="5" t="s">
         <v>310</v>
       </c>
       <c r="C105" s="2">
         <v>3</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E105" s="6" t="s">
+      <c r="D105" s="16">
+        <v>44201</v>
+      </c>
+      <c r="E105" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="F105" s="6" t="s">
+      <c r="F105" s="5" t="s">
         <v>430</v>
       </c>
       <c r="G105" s="2">
         <v>7785281</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="J105" s="4" t="s">
+      <c r="J105" s="3" t="s">
         <v>591</v>
       </c>
     </row>
@@ -7322,26 +7325,26 @@
       <c r="A106" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B106" s="6" t="s">
+      <c r="B106" s="5" t="s">
         <v>313</v>
       </c>
       <c r="C106" s="2">
         <v>3</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E106" s="6" t="s">
+      <c r="D106" s="16">
+        <v>44361</v>
+      </c>
+      <c r="E106" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="F106" s="15" t="s">
+      <c r="F106" s="12" t="s">
         <v>431</v>
       </c>
       <c r="G106" s="2">
         <v>8201440</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>527</v>
@@ -7354,31 +7357,31 @@
       <c r="A107" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="5" t="s">
         <v>316</v>
       </c>
       <c r="C107" s="2">
         <v>9</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E107" s="6" t="s">
+      <c r="D107" s="16">
+        <v>44228</v>
+      </c>
+      <c r="E107" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F107" s="6" t="s">
+      <c r="F107" s="5" t="s">
         <v>432</v>
       </c>
       <c r="G107" s="2">
         <v>7852071</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="J107" s="4" t="s">
+      <c r="J107" s="3" t="s">
         <v>624</v>
       </c>
     </row>
@@ -7386,31 +7389,31 @@
       <c r="A108" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B108" s="6" t="s">
+      <c r="B108" s="5" t="s">
         <v>319</v>
       </c>
       <c r="C108" s="2">
         <v>6</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E108" s="6" t="s">
+      <c r="D108" s="16">
+        <v>44136</v>
+      </c>
+      <c r="E108" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="F108" s="6" t="s">
+      <c r="F108" s="5" t="s">
         <v>433</v>
       </c>
       <c r="G108" s="2">
         <v>7603994</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="J108" s="4" t="s">
+      <c r="J108" s="3" t="s">
         <v>625</v>
       </c>
     </row>
@@ -7418,26 +7421,26 @@
       <c r="A109" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="5" t="s">
         <v>322</v>
       </c>
       <c r="C109" s="2">
         <v>5</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E109" s="6" t="s">
+      <c r="D109" s="16">
+        <v>44463</v>
+      </c>
+      <c r="E109" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="F109" s="13" t="s">
+      <c r="F109" s="10" t="s">
         <v>434</v>
       </c>
       <c r="G109" s="2">
         <v>8462638</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>530</v>
@@ -7450,26 +7453,26 @@
       <c r="A110" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B110" s="6" t="s">
+      <c r="B110" s="5" t="s">
         <v>325</v>
       </c>
       <c r="C110" s="2">
         <v>4</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E110" s="6" t="s">
+      <c r="D110" s="16">
+        <v>44180</v>
+      </c>
+      <c r="E110" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="F110" s="6" t="s">
+      <c r="F110" s="5" t="s">
         <v>435</v>
       </c>
       <c r="G110" s="2">
         <v>7745997</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>531</v>
@@ -7482,31 +7485,31 @@
       <c r="A111" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B111" s="6" t="s">
+      <c r="B111" s="5" t="s">
         <v>328</v>
       </c>
       <c r="C111" s="2">
         <v>1</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E111" s="6" t="s">
+      <c r="D111" s="16">
+        <v>44309</v>
+      </c>
+      <c r="E111" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="F111" s="15" t="s">
+      <c r="F111" s="12" t="s">
         <v>436</v>
       </c>
       <c r="G111" s="2">
         <v>8064424</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="J111" s="4" t="s">
+      <c r="J111" s="3" t="s">
         <v>628</v>
       </c>
     </row>
@@ -7514,16 +7517,16 @@
       <c r="A112" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B112" s="6" t="s">
+      <c r="B112" s="5" t="s">
         <v>331</v>
       </c>
       <c r="C112" s="2">
         <v>6</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="E112" s="6" t="s">
+      <c r="D112" s="16">
+        <v>44334</v>
+      </c>
+      <c r="E112" s="5" t="s">
         <v>332</v>
       </c>
       <c r="F112" s="1" t="s">
@@ -7533,12 +7536,12 @@
         <v>8128982</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="J112" s="4" t="s">
+      <c r="J112" s="3" t="s">
         <v>629</v>
       </c>
     </row>

</xml_diff>